<commit_message>
Add tab for summaries
</commit_message>
<xml_diff>
--- a/results/forecast_tables.xlsx
+++ b/results/forecast_tables.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA95106-99E9-4427-ACAD-B2764D5FE354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53748542-FE63-42F0-9821-1E2BED5AAF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="-12000" windowWidth="14325" windowHeight="7245" activeTab="2" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>Species</t>
   </si>
@@ -241,6 +242,51 @@
   </si>
   <si>
     <t>We have a couple things going on here: 1 is that the movement of spawning grounds may lead to spawning in areas that have unfavorable currents meaning that eggs and larvae don't get transported to suitable nursery habitat. This means fewer fish surviving to the juvenile phase and therefore the adult phase. So for species with high commerical importance this mean less availability. For some species, there is also already targeted fishing for spawning aggregations, so there may be a shift to new fishing grounds during different times of the year</t>
+  </si>
+  <si>
+    <t>CESM</t>
+  </si>
+  <si>
+    <t>GFDL</t>
+  </si>
+  <si>
+    <t>MIROC</t>
+  </si>
+  <si>
+    <t>PCOD</t>
+  </si>
+  <si>
+    <t>YFS</t>
+  </si>
+  <si>
+    <t>NRS</t>
+  </si>
+  <si>
+    <t>AKP egg</t>
+  </si>
+  <si>
+    <t>AKP larvae</t>
+  </si>
+  <si>
+    <t>FHS egg</t>
+  </si>
+  <si>
+    <t>FHS larvae</t>
+  </si>
+  <si>
+    <t>WP egg</t>
+  </si>
+  <si>
+    <t>WP larvae</t>
+  </si>
+  <si>
+    <t>Shows lower aundance in the northern area in comparison, concentrated along islands</t>
+  </si>
+  <si>
+    <t>Shows two spots with high abundance</t>
+  </si>
+  <si>
+    <t>Shows two spots with high abundance but more diffuse in the northern area in comparison</t>
   </si>
 </sst>
 </file>
@@ -522,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -542,51 +588,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -726,11 +727,56 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -752,7 +798,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01F31920-3675-40CB-A0B5-C656B855E1F3}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01F31920-3675-40CB-A0B5-C656B855E1F3}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6">
   <autoFilter ref="A1:E10" xr:uid="{01F31920-3675-40CB-A0B5-C656B855E1F3}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -761,11 +807,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{59748C80-9906-44AA-A9DE-63F6C5A439D8}" name="Species" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DBE80379-BFF1-47EB-B68C-AA0E494BCF9B}" name="Life stage" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{98DD0F98-13FB-4597-B680-E021227D985C}" name="Δ in abundance" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A2FD5BDB-A58A-4D7B-ACBE-EF3A9ECE04A0}" name="Δ in location" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E8001350-0352-4634-AC57-53336B1A5D97}" name="Δ spawn timing" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{59748C80-9906-44AA-A9DE-63F6C5A439D8}" name="Species" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DBE80379-BFF1-47EB-B68C-AA0E494BCF9B}" name="Life stage" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{98DD0F98-13FB-4597-B680-E021227D985C}" name="Δ in abundance" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A2FD5BDB-A58A-4D7B-ACBE-EF3A9ECE04A0}" name="Δ in location" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E8001350-0352-4634-AC57-53336B1A5D97}" name="Δ spawn timing" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1475,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31F9ACA-ACD1-4BF9-8FA4-0BE2738B7507}">
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1552,4 +1598,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837DD457-1957-4AAB-A625-B20786D6AEC1}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update table with summary descriptions
</commit_message>
<xml_diff>
--- a/results/forecast_tables.xlsx
+++ b/results/forecast_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53748542-FE63-42F0-9821-1E2BED5AAF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01CC872-B073-4C0F-911B-966721AF0A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
   <si>
     <t>Species</t>
   </si>
@@ -287,6 +287,117 @@
   </si>
   <si>
     <t>Shows two spots with high abundance but more diffuse in the northern area in comparison</t>
+  </si>
+  <si>
+    <t>SSP1-2.6</t>
+  </si>
+  <si>
+    <t>SSP5-8.5</t>
+  </si>
+  <si>
+    <t>Little change</t>
+  </si>
+  <si>
+    <t>More contraction of high density areas, particularly in the northern concentration</t>
+  </si>
+  <si>
+    <t>More contraction with middle and late century compared to others</t>
+  </si>
+  <si>
+    <t>Similar to MIROC</t>
+  </si>
+  <si>
+    <t>In some cases, more contraction than high emission scenario</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Contraction at specific sites (northwestern corner, near Aleutians)</t>
+  </si>
+  <si>
+    <t>Contraction toward the southeast, further to the inner shelf</t>
+  </si>
+  <si>
+    <t>Sometimes slightly less contraction by end of century</t>
+  </si>
+  <si>
+    <t>Broad but concentrated densities near AK peninsula peaking at mid-century</t>
+  </si>
+  <si>
+    <t>Concentrations near AK peninsula and also north of Pribs</t>
+  </si>
+  <si>
+    <t>Concentrated density at Unimak Pass but some more spread out over the other two hot spots</t>
+  </si>
+  <si>
+    <t>Higher densities toward end of century</t>
+  </si>
+  <si>
+    <t>Higher densities at mid-centuries</t>
+  </si>
+  <si>
+    <t>Over time there is a spreading of densities across the mid-shelf focused near the AK peninsula but faintly north of the Pribs</t>
+  </si>
+  <si>
+    <t>Reduction over the course of the century</t>
+  </si>
+  <si>
+    <t>Typically smaller area of high density at beginning of century in comparison</t>
+  </si>
+  <si>
+    <t>Wider concentration of high density in comparison, but mid and late century look pretty much the same for both scenarios</t>
+  </si>
+  <si>
+    <t>Reduction in size of area with high densities of eggs</t>
+  </si>
+  <si>
+    <t>Increase in area of high densities over course of century but the area near the AK peninsula reduces by quite a bit</t>
+  </si>
+  <si>
+    <t>High density near AK peninsula but switches to northern shelf over mid and late century</t>
+  </si>
+  <si>
+    <t>Shift from higher densities in south to northern shelf</t>
+  </si>
+  <si>
+    <t>Highest densities in northern area show up in late century</t>
+  </si>
+  <si>
+    <t>High densities start to show up in mid-century</t>
+  </si>
+  <si>
+    <t>Western cluster disappears, but pattern in high densities differs for scenario</t>
+  </si>
+  <si>
+    <t>Similar reduction in density over time for both scenarios</t>
+  </si>
+  <si>
+    <t>Similar to CESM with opposite responses but the western cluster doesn't disappear entirely</t>
+  </si>
+  <si>
+    <t>Usually a reduction in density over time with western cluster all but disappearing in all cases</t>
+  </si>
+  <si>
+    <t>Some increase in density by end of century on mid-shelf</t>
+  </si>
+  <si>
+    <t>Concentrations to the west seem to disappear or reduce over century, high density cluster shows up in some situations, possible problematic isolated cluster below St Matthew</t>
+  </si>
+  <si>
+    <t>Problems with this one, no patterns showing</t>
+  </si>
+  <si>
+    <t>Reduction in density across shelf over century but cluster near Unimak Pass stays strong, band of density across the northern shelf seems to narrow over time</t>
+  </si>
+  <si>
+    <t>Reduction over century, high density near Unimak Pass consistent but shrinks</t>
+  </si>
+  <si>
+    <t>Reduction over century, high density near Unimak Pass consistent but shrinks though less than CESM</t>
+  </si>
+  <si>
+    <t>Similar amongst scenarios, most differences seen for specific ESMs during mid-century</t>
   </si>
 </sst>
 </file>
@@ -1602,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837DD457-1957-4AAB-A625-B20786D6AEC1}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1621,82 +1732,235 @@
     <col min="10" max="10" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="166" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add COG tab, reorganize other tabs
</commit_message>
<xml_diff>
--- a/results/forecast_tables.xlsx
+++ b/results/forecast_tables.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17F73B9-1624-4766-8945-F72142B28E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F192847C-C1F3-497E-9882-1249A106EA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Summary Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Species Descriptions" sheetId="2" r:id="rId2"/>
+    <sheet name="COG Tables" sheetId="5" r:id="rId3"/>
+    <sheet name="Detailed Observations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
   <si>
     <t>Species</t>
   </si>
@@ -145,18 +145,6 @@
     <t>geography</t>
   </si>
   <si>
-    <t>Do we know how each species does with warmer temperatures?</t>
-  </si>
-  <si>
-    <t>Cod: Hatch success declines above 4-5 C</t>
-  </si>
-  <si>
-    <t>How do we plan to look at change over time?</t>
-  </si>
-  <si>
-    <t>What will we do with the results in terms of management?</t>
-  </si>
-  <si>
     <t>decrease/increase</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
     <t>temperature</t>
   </si>
   <si>
-    <t>How does spawn timing relate to the results?</t>
-  </si>
-  <si>
     <t>Egg type</t>
   </si>
   <si>
@@ -205,39 +190,6 @@
     <t>benthic</t>
   </si>
   <si>
-    <t>Species for which the flexible geography model was selected spawn later and on the mid to inner portion of the shelf</t>
-  </si>
-  <si>
-    <t>A local overlap index, similar to how predator-prey overlap is looked at, in order to quantify what change and in what direction that is occurring</t>
-  </si>
-  <si>
-    <t>Explain the variable coefficient terms and why they are used</t>
-  </si>
-  <si>
-    <t>This research is helpful in determining the vulnerability of species to climate change. It also complements what the Alaska Climate Integrated Modeling Project is doing currently with adult fish, and can inform management of fish in the long term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The variable coefficient terms essentially allow timing of spawning or location of spawning to vary with mean sea surface temperature. So, we calculated what was basically a temperature index, or an average temperature for a portion of the shelf </t>
-  </si>
-  <si>
-    <t>How deep are they sampling</t>
-  </si>
-  <si>
-    <t>200 m or 10 m off the bottom using bongo nets</t>
-  </si>
-  <si>
-    <t>Why do you think you see the opposite response for pollock eggs and larvae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What we see in the smooth term curves is that at about 3 degrees we start to get a decline in eggs while for larvae, there is in increase up to 4 degrees and no decline until about 8 degrees. </t>
-  </si>
-  <si>
-    <t>Which are the main economic implications of the new areas for spawning of these species? and do you think coupling the eggs/larval models would be a useful step for the forecasts?</t>
-  </si>
-  <si>
-    <t>We have a couple things going on here: 1 is that the movement of spawning grounds may lead to spawning in areas that have unfavorable currents meaning that eggs and larvae don't get transported to suitable nursery habitat. This means fewer fish surviving to the juvenile phase and therefore the adult phase. So for species with high commerical importance this mean less availability. For some species, there is also already targeted fishing for spawning aggregations, so there may be a shift to new fishing grounds during different times of the year</t>
-  </si>
-  <si>
     <t>CESM</t>
   </si>
   <si>
@@ -425,13 +377,43 @@
   </si>
   <si>
     <t>SE</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Avgerage Movement</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Time Period</t>
+  </si>
+  <si>
+    <t>Hindcast</t>
+  </si>
+  <si>
+    <t>Flathead Sole</t>
+  </si>
+  <si>
+    <t>Alaska Plaice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,8 +453,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +477,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -694,20 +707,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -755,63 +847,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -928,10 +964,10 @@
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{59748C80-9906-44AA-A9DE-63F6C5A439D8}" name="Species" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DBE80379-BFF1-47EB-B68C-AA0E494BCF9B}" name="Life stage" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{98DD0F98-13FB-4597-B680-E021227D985C}" name="Δ in abundance" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DBE80379-BFF1-47EB-B68C-AA0E494BCF9B}" name="Life stage" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{98DD0F98-13FB-4597-B680-E021227D985C}" name="Δ in abundance" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{A2FD5BDB-A58A-4D7B-ACBE-EF3A9ECE04A0}" name="Δ in location" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{E8001350-0352-4634-AC57-53336B1A5D97}" name="Δ spawn timing" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{E8001350-0352-4634-AC57-53336B1A5D97}" name="Δ spawn timing" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1237,7 +1273,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>11</v>
@@ -1292,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>11</v>
@@ -1307,10 +1343,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>19</v>
@@ -1322,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>11</v>
@@ -1337,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>12</v>
@@ -1352,10 +1388,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -1367,10 +1403,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>19</v>
@@ -1384,10 +1420,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>19</v>
@@ -1401,7 +1437,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>11</v>
@@ -1424,7 +1460,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,10 +1483,10 @@
         <v>17</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>20</v>
@@ -1476,19 +1512,19 @@
         <v>22</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>32</v>
@@ -1505,19 +1541,19 @@
         <v>25</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>32</v>
@@ -1534,17 +1570,17 @@
         <v>26</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>43</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>33</v>
@@ -1561,17 +1597,17 @@
         <v>29</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>34</v>
@@ -1588,10 +1624,10 @@
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
@@ -1615,10 +1651,10 @@
         <v>30</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18" t="s">
@@ -1638,85 +1674,339 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31F9ACA-ACD1-4BF9-8FA4-0BE2738B7507}">
-  <dimension ref="A2:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC51D1-50FC-4EC8-953A-F70BFC92C4CF}">
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.36328125" customWidth="1"/>
-    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>65</v>
-      </c>
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="33">
+        <v>91.3</v>
+      </c>
+      <c r="E2" s="33">
+        <v>35.1</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="40">
+        <v>50.8</v>
+      </c>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="33">
+        <v>49.6</v>
+      </c>
+      <c r="E3" s="33">
+        <v>25</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="38">
+        <v>1</v>
+      </c>
+      <c r="J3" s="42">
+        <v>64.8</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="35">
+        <v>79.5</v>
+      </c>
+      <c r="E4" s="35">
+        <v>26.9</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="38">
+        <v>2</v>
+      </c>
+      <c r="J4" s="40">
+        <v>32.9</v>
+      </c>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="35">
+        <v>32.9</v>
+      </c>
+      <c r="E5" s="35">
+        <v>21.8</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="38">
+        <v>3</v>
+      </c>
+      <c r="J5" s="40">
+        <v>26.7</v>
+      </c>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="33">
+        <v>43.2</v>
+      </c>
+      <c r="E6" s="33">
+        <v>21.7</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="40">
+        <v>27.7</v>
+      </c>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="33">
+        <v>99.9</v>
+      </c>
+      <c r="E7" s="33">
+        <v>49.6</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="38">
+        <v>1</v>
+      </c>
+      <c r="J7" s="40">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="35">
+        <v>235.4</v>
+      </c>
+      <c r="E8" s="35">
+        <v>80.3</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="38">
+        <v>2</v>
+      </c>
+      <c r="J8" s="40">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="35">
+        <v>93.6</v>
+      </c>
+      <c r="E9" s="35">
+        <v>50.3</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="38">
+        <v>3</v>
+      </c>
+      <c r="J9" s="42">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="33">
+        <v>5.4</v>
+      </c>
+      <c r="E10" s="33">
+        <v>4.8</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="41">
+        <v>176.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H11" s="31"/>
+      <c r="I11" s="38">
+        <v>1</v>
+      </c>
+      <c r="J11" s="42">
+        <v>206.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H12" s="31"/>
+      <c r="I12" s="38">
+        <v>2</v>
+      </c>
+      <c r="J12" s="41">
+        <v>168.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H13" s="31"/>
+      <c r="I13" s="38">
+        <v>3</v>
+      </c>
+      <c r="J13" s="41">
+        <v>126.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I16" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1724,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837DD457-1957-4AAB-A625-B20786D6AEC1}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1743,130 +2033,130 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1883,67 +2173,67 @@
     </row>
     <row r="6" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1960,34 +2250,34 @@
     </row>
     <row r="9" spans="1:11" ht="166" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="K9" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update COG figures and tables
</commit_message>
<xml_diff>
--- a/results/forecast_tables.xlsx
+++ b/results/forecast_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D78EFFB-1686-4FD4-8BA0-155C68F3A91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB529E7-4EBA-4209-90D0-813C46B31E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{DED94058-4F82-4D89-AF80-6EFA57D45485}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Table" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="127">
   <si>
     <t>Species</t>
   </si>
@@ -404,6 +404,21 @@
   </si>
   <si>
     <t>Average Movement</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2015-2039</t>
+  </si>
+  <si>
+    <t>2040-2069</t>
+  </si>
+  <si>
+    <t>2070-2099</t>
   </si>
 </sst>
 </file>
@@ -413,7 +428,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +481,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -482,19 +503,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF6A37A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FF78E9F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,27 +739,29 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +961,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF78E9F8"/>
       <color rgb="FFF6A37A"/>
-      <color rgb="FF78E9F8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1675,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC51D1-50FC-4EC8-953A-F70BFC92C4CF}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:R162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1692,9 +1715,13 @@
     <col min="8" max="8" width="16.7265625" customWidth="1"/>
     <col min="9" max="9" width="13.7265625" customWidth="1"/>
     <col min="10" max="10" width="11.7265625" customWidth="1"/>
+    <col min="14" max="14" width="17.1796875" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" customWidth="1"/>
+    <col min="17" max="17" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1712,297 +1739,1516 @@
       </c>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="34" t="s">
         <v>114</v>
       </c>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+      <c r="N1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="33">
-        <v>91.3</v>
-      </c>
-      <c r="E2" s="33">
-        <v>35.1</v>
+      <c r="C2" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="36">
+        <v>105.1</v>
+      </c>
+      <c r="E2" s="36">
+        <v>40.700000000000003</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="40">
-        <v>50.8</v>
-      </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32" t="s">
+      <c r="J2" s="36">
+        <v>55.5</v>
+      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="N2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="38">
+        <v>151.69999999999999</v>
+      </c>
+      <c r="R2" s="37"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="33">
-        <v>49.6</v>
-      </c>
-      <c r="E3" s="33">
-        <v>25</v>
+      <c r="C3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="36">
+        <v>58.3</v>
+      </c>
+      <c r="E3" s="36">
+        <v>24.9</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="38">
-        <v>1</v>
-      </c>
-      <c r="J3" s="42">
+      <c r="H3" s="31"/>
+      <c r="I3" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="35">
         <v>64.8</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="39">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="R3" s="37"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="35">
-        <v>79.5</v>
-      </c>
-      <c r="E4" s="35">
-        <v>26.9</v>
+      <c r="C4" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="36">
+        <v>71.5</v>
+      </c>
+      <c r="E4" s="36">
+        <v>24.1</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="38">
-        <v>2</v>
-      </c>
-      <c r="J4" s="40">
+      <c r="H4" s="31"/>
+      <c r="I4" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="36">
         <v>32.9</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="R4" s="37"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="35">
-        <v>32.9</v>
-      </c>
-      <c r="E5" s="35">
-        <v>21.8</v>
+      <c r="D5" s="36">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E5" s="36">
+        <v>22.4</v>
       </c>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="38">
+      <c r="H5" s="31"/>
+      <c r="I5" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="36">
+        <v>26.7</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="N5" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q5" s="39">
+        <v>104.1</v>
+      </c>
+      <c r="R5" s="37"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="40">
-        <v>26.7</v>
-      </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="33">
-        <v>43.2</v>
-      </c>
-      <c r="E6" s="33">
-        <v>21.7</v>
+      <c r="C6" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="36">
+        <v>41.9</v>
+      </c>
+      <c r="E6" s="36">
+        <v>25.8</v>
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="J6" s="40">
-        <v>27.7</v>
-      </c>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32" t="s">
+      <c r="J6" s="36">
+        <v>33.4</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q6" s="39">
+        <v>90.2</v>
+      </c>
+      <c r="R6" s="37"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="33">
-        <v>99.9</v>
-      </c>
-      <c r="E7" s="33">
-        <v>49.6</v>
+      <c r="D7" s="36">
+        <v>82.6</v>
+      </c>
+      <c r="E7" s="36">
+        <v>46.6</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
-      <c r="I7" s="38">
-        <v>1</v>
-      </c>
-      <c r="J7" s="40">
+      <c r="I7" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="36">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>31.9</v>
+      </c>
+      <c r="R7" s="37"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="35">
-        <v>235.4</v>
-      </c>
-      <c r="E8" s="35">
-        <v>80.3</v>
+      <c r="D8" s="36">
+        <v>281.60000000000002</v>
+      </c>
+      <c r="E8" s="36">
+        <v>94.2</v>
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
-      <c r="I8" s="38">
-        <v>2</v>
-      </c>
-      <c r="J8" s="40">
+      <c r="I8" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="36">
         <v>49.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+      <c r="N8" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q8" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="R8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="35">
-        <v>93.6</v>
-      </c>
-      <c r="E9" s="35">
-        <v>50.3</v>
+      <c r="D9" s="36">
+        <v>97.9</v>
+      </c>
+      <c r="E9" s="36">
+        <v>47.9</v>
       </c>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="38">
-        <v>3</v>
-      </c>
-      <c r="J9" s="42">
+      <c r="I9" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="J9" s="35">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="R9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="33">
-        <v>5.4</v>
-      </c>
-      <c r="E10" s="33">
-        <v>4.8</v>
+      <c r="C10" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="36">
+        <v>5</v>
+      </c>
+      <c r="E10" s="36">
+        <v>6.2</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="J10" s="41">
-        <v>176.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J10" s="35">
+        <v>206.6</v>
+      </c>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="H11" s="31"/>
-      <c r="I11" s="38">
-        <v>1</v>
-      </c>
-      <c r="J11" s="42">
+      <c r="I11" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="36">
         <v>206.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N11" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q11" s="33">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="R11" s="37"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="H12" s="31"/>
-      <c r="I12" s="38">
-        <v>2</v>
-      </c>
-      <c r="J12" s="41">
+      <c r="I12" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="36">
         <v>168.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q12" s="33">
+        <v>58.9</v>
+      </c>
+      <c r="R12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="H13" s="31"/>
-      <c r="I13" s="38">
+      <c r="I13" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="36">
+        <v>126.8</v>
+      </c>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q13" s="33">
+        <v>59</v>
+      </c>
+      <c r="R13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I14" s="26"/>
+      <c r="N14" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="41">
-        <v>126.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P14" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" s="33">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="R14" s="37"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q15" s="33">
+        <v>53.1</v>
+      </c>
+      <c r="R15" s="37"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="I16" s="26"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q16" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="R16" s="37"/>
+    </row>
+    <row r="17" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N17" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q17" s="33">
+        <v>236</v>
+      </c>
+      <c r="R17" s="37"/>
+    </row>
+    <row r="18" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q18" s="33">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="R18" s="37"/>
+    </row>
+    <row r="19" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q19" s="33">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="R19" s="37"/>
+    </row>
+    <row r="20" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N20" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q20" s="33">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="R20" s="37"/>
+    </row>
+    <row r="21" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q21" s="33">
+        <v>407.2</v>
+      </c>
+      <c r="R21" s="37"/>
+    </row>
+    <row r="22" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q22" s="33">
+        <v>642.6</v>
+      </c>
+      <c r="R22" s="37"/>
+    </row>
+    <row r="23" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N23" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P23" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q23" s="33">
+        <v>35.6</v>
+      </c>
+      <c r="R23" s="37"/>
+    </row>
+    <row r="24" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q24" s="33">
+        <v>134.6</v>
+      </c>
+      <c r="R24" s="37"/>
+    </row>
+    <row r="25" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q25" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="R25" s="37"/>
+    </row>
+    <row r="26" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N26" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q26" s="33">
+        <v>56.4</v>
+      </c>
+      <c r="R26" s="37"/>
+    </row>
+    <row r="27" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q27" s="33">
+        <v>108.4</v>
+      </c>
+      <c r="R27" s="37"/>
+    </row>
+    <row r="28" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q28" s="33">
+        <v>120.1</v>
+      </c>
+      <c r="R28" s="37"/>
+    </row>
+    <row r="29" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+    </row>
+    <row r="30" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+    </row>
+    <row r="31" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+    </row>
+    <row r="32" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+    </row>
+    <row r="33" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+    </row>
+    <row r="34" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="37"/>
+    </row>
+    <row r="35" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+    </row>
+    <row r="36" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="37"/>
+    </row>
+    <row r="37" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+    </row>
+    <row r="38" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="37"/>
+    </row>
+    <row r="39" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+    </row>
+    <row r="40" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="37"/>
+      <c r="R40" s="37"/>
+    </row>
+    <row r="41" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+    </row>
+    <row r="42" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+    </row>
+    <row r="43" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+    </row>
+    <row r="44" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+    </row>
+    <row r="45" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+    </row>
+    <row r="46" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+    </row>
+    <row r="47" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+    </row>
+    <row r="48" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+    </row>
+    <row r="49" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+    </row>
+    <row r="50" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+    </row>
+    <row r="51" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N51" s="31"/>
+      <c r="O51" s="31"/>
+      <c r="P51" s="31"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+    </row>
+    <row r="52" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N52" s="31"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
+    </row>
+    <row r="53" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N53" s="31"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="31"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+    </row>
+    <row r="54" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N54" s="31"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="31"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+    </row>
+    <row r="55" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+    </row>
+    <row r="56" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N56" s="31"/>
+      <c r="O56" s="31"/>
+      <c r="P56" s="31"/>
+      <c r="Q56" s="37"/>
+      <c r="R56" s="37"/>
+    </row>
+    <row r="57" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N57" s="31"/>
+      <c r="O57" s="31"/>
+      <c r="P57" s="31"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+    </row>
+    <row r="58" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
+      <c r="Q58" s="37"/>
+      <c r="R58" s="37"/>
+    </row>
+    <row r="59" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+    </row>
+    <row r="60" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
+      <c r="P60" s="31"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="37"/>
+    </row>
+    <row r="61" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N61" s="31"/>
+      <c r="O61" s="31"/>
+      <c r="P61" s="31"/>
+      <c r="Q61" s="37"/>
+      <c r="R61" s="37"/>
+    </row>
+    <row r="62" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N62" s="31"/>
+      <c r="O62" s="31"/>
+      <c r="P62" s="31"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+    </row>
+    <row r="63" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N63" s="31"/>
+      <c r="O63" s="31"/>
+      <c r="P63" s="31"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+    </row>
+    <row r="64" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N64" s="31"/>
+      <c r="O64" s="31"/>
+      <c r="P64" s="31"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+    </row>
+    <row r="65" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N65" s="31"/>
+      <c r="O65" s="31"/>
+      <c r="P65" s="31"/>
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+    </row>
+    <row r="66" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N66" s="31"/>
+      <c r="O66" s="31"/>
+      <c r="P66" s="31"/>
+      <c r="Q66" s="37"/>
+      <c r="R66" s="37"/>
+    </row>
+    <row r="67" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N67" s="31"/>
+      <c r="O67" s="31"/>
+      <c r="P67" s="31"/>
+      <c r="Q67" s="37"/>
+      <c r="R67" s="37"/>
+    </row>
+    <row r="68" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N68" s="31"/>
+      <c r="O68" s="31"/>
+      <c r="P68" s="31"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+    </row>
+    <row r="69" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N69" s="31"/>
+      <c r="O69" s="31"/>
+      <c r="P69" s="31"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="37"/>
+    </row>
+    <row r="70" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N70" s="31"/>
+      <c r="O70" s="31"/>
+      <c r="P70" s="31"/>
+      <c r="Q70" s="37"/>
+      <c r="R70" s="37"/>
+    </row>
+    <row r="71" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N71" s="31"/>
+      <c r="O71" s="31"/>
+      <c r="P71" s="31"/>
+      <c r="Q71" s="37"/>
+      <c r="R71" s="37"/>
+    </row>
+    <row r="72" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N72" s="31"/>
+      <c r="O72" s="31"/>
+      <c r="P72" s="31"/>
+      <c r="Q72" s="37"/>
+      <c r="R72" s="37"/>
+    </row>
+    <row r="73" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N73" s="31"/>
+      <c r="O73" s="31"/>
+      <c r="P73" s="31"/>
+      <c r="Q73" s="37"/>
+      <c r="R73" s="37"/>
+    </row>
+    <row r="74" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N74" s="31"/>
+      <c r="O74" s="31"/>
+      <c r="P74" s="31"/>
+      <c r="Q74" s="37"/>
+      <c r="R74" s="37"/>
+    </row>
+    <row r="75" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N75" s="31"/>
+      <c r="O75" s="31"/>
+      <c r="P75" s="31"/>
+      <c r="Q75" s="37"/>
+      <c r="R75" s="37"/>
+    </row>
+    <row r="76" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N76" s="31"/>
+      <c r="O76" s="31"/>
+      <c r="P76" s="31"/>
+      <c r="Q76" s="37"/>
+      <c r="R76" s="37"/>
+    </row>
+    <row r="77" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N77" s="31"/>
+      <c r="O77" s="31"/>
+      <c r="P77" s="31"/>
+      <c r="Q77" s="37"/>
+      <c r="R77" s="37"/>
+    </row>
+    <row r="78" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N78" s="31"/>
+      <c r="O78" s="31"/>
+      <c r="P78" s="31"/>
+      <c r="Q78" s="37"/>
+      <c r="R78" s="37"/>
+    </row>
+    <row r="79" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N79" s="31"/>
+      <c r="O79" s="31"/>
+      <c r="P79" s="31"/>
+      <c r="Q79" s="37"/>
+      <c r="R79" s="37"/>
+    </row>
+    <row r="80" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N80" s="31"/>
+      <c r="O80" s="31"/>
+      <c r="P80" s="31"/>
+      <c r="Q80" s="37"/>
+      <c r="R80" s="37"/>
+    </row>
+    <row r="81" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N81" s="31"/>
+      <c r="O81" s="31"/>
+      <c r="P81" s="31"/>
+      <c r="Q81" s="37"/>
+      <c r="R81" s="37"/>
+    </row>
+    <row r="82" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N82" s="31"/>
+      <c r="O82" s="31"/>
+      <c r="P82" s="31"/>
+      <c r="Q82" s="37"/>
+      <c r="R82" s="37"/>
+    </row>
+    <row r="83" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N83" s="31"/>
+      <c r="O83" s="31"/>
+      <c r="P83" s="31"/>
+      <c r="Q83" s="37"/>
+      <c r="R83" s="37"/>
+    </row>
+    <row r="84" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N84" s="31"/>
+      <c r="O84" s="31"/>
+      <c r="P84" s="31"/>
+      <c r="Q84" s="37"/>
+      <c r="R84" s="37"/>
+    </row>
+    <row r="85" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N85" s="31"/>
+      <c r="O85" s="31"/>
+      <c r="P85" s="31"/>
+      <c r="Q85" s="37"/>
+      <c r="R85" s="37"/>
+    </row>
+    <row r="86" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N86" s="31"/>
+      <c r="O86" s="31"/>
+      <c r="P86" s="31"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="37"/>
+    </row>
+    <row r="87" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N87" s="31"/>
+      <c r="O87" s="31"/>
+      <c r="P87" s="31"/>
+      <c r="Q87" s="37"/>
+      <c r="R87" s="37"/>
+    </row>
+    <row r="88" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N88" s="31"/>
+      <c r="O88" s="31"/>
+      <c r="P88" s="31"/>
+      <c r="Q88" s="37"/>
+      <c r="R88" s="37"/>
+    </row>
+    <row r="89" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N89" s="31"/>
+      <c r="O89" s="31"/>
+      <c r="P89" s="31"/>
+      <c r="Q89" s="37"/>
+      <c r="R89" s="37"/>
+    </row>
+    <row r="90" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N90" s="31"/>
+      <c r="O90" s="31"/>
+      <c r="P90" s="31"/>
+      <c r="Q90" s="37"/>
+      <c r="R90" s="37"/>
+    </row>
+    <row r="91" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N91" s="31"/>
+      <c r="O91" s="31"/>
+      <c r="P91" s="31"/>
+      <c r="Q91" s="37"/>
+      <c r="R91" s="37"/>
+    </row>
+    <row r="92" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N92" s="31"/>
+      <c r="O92" s="31"/>
+      <c r="P92" s="31"/>
+      <c r="Q92" s="37"/>
+      <c r="R92" s="37"/>
+    </row>
+    <row r="93" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N93" s="31"/>
+      <c r="O93" s="31"/>
+      <c r="P93" s="31"/>
+      <c r="Q93" s="37"/>
+      <c r="R93" s="37"/>
+    </row>
+    <row r="94" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N94" s="31"/>
+      <c r="O94" s="31"/>
+      <c r="P94" s="31"/>
+      <c r="Q94" s="37"/>
+      <c r="R94" s="37"/>
+    </row>
+    <row r="95" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N95" s="31"/>
+      <c r="O95" s="31"/>
+      <c r="P95" s="31"/>
+      <c r="Q95" s="37"/>
+      <c r="R95" s="37"/>
+    </row>
+    <row r="96" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N96" s="31"/>
+      <c r="O96" s="31"/>
+      <c r="P96" s="31"/>
+      <c r="Q96" s="37"/>
+      <c r="R96" s="37"/>
+    </row>
+    <row r="97" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N97" s="31"/>
+      <c r="O97" s="31"/>
+      <c r="P97" s="31"/>
+      <c r="Q97" s="37"/>
+      <c r="R97" s="37"/>
+    </row>
+    <row r="98" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N98" s="31"/>
+      <c r="O98" s="31"/>
+      <c r="P98" s="31"/>
+      <c r="Q98" s="37"/>
+      <c r="R98" s="37"/>
+    </row>
+    <row r="99" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N99" s="31"/>
+      <c r="O99" s="31"/>
+      <c r="P99" s="31"/>
+      <c r="Q99" s="37"/>
+      <c r="R99" s="37"/>
+    </row>
+    <row r="100" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N100" s="31"/>
+      <c r="O100" s="31"/>
+      <c r="P100" s="31"/>
+      <c r="Q100" s="37"/>
+      <c r="R100" s="37"/>
+    </row>
+    <row r="101" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N101" s="31"/>
+      <c r="O101" s="31"/>
+      <c r="P101" s="31"/>
+      <c r="Q101" s="37"/>
+      <c r="R101" s="37"/>
+    </row>
+    <row r="102" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N102" s="31"/>
+      <c r="O102" s="31"/>
+      <c r="P102" s="31"/>
+      <c r="Q102" s="37"/>
+      <c r="R102" s="37"/>
+    </row>
+    <row r="103" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N103" s="31"/>
+      <c r="O103" s="31"/>
+      <c r="P103" s="31"/>
+      <c r="Q103" s="37"/>
+      <c r="R103" s="37"/>
+    </row>
+    <row r="104" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N104" s="31"/>
+      <c r="O104" s="31"/>
+      <c r="P104" s="31"/>
+      <c r="Q104" s="37"/>
+      <c r="R104" s="37"/>
+    </row>
+    <row r="105" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N105" s="31"/>
+      <c r="O105" s="31"/>
+      <c r="P105" s="31"/>
+      <c r="Q105" s="37"/>
+      <c r="R105" s="37"/>
+    </row>
+    <row r="106" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N106" s="31"/>
+      <c r="O106" s="31"/>
+      <c r="P106" s="31"/>
+      <c r="Q106" s="37"/>
+      <c r="R106" s="37"/>
+    </row>
+    <row r="107" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N107" s="31"/>
+      <c r="O107" s="31"/>
+      <c r="P107" s="31"/>
+      <c r="Q107" s="37"/>
+      <c r="R107" s="37"/>
+    </row>
+    <row r="108" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N108" s="31"/>
+      <c r="O108" s="31"/>
+      <c r="P108" s="31"/>
+      <c r="Q108" s="37"/>
+      <c r="R108" s="37"/>
+    </row>
+    <row r="109" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N109" s="31"/>
+      <c r="O109" s="31"/>
+      <c r="P109" s="31"/>
+      <c r="Q109" s="37"/>
+      <c r="R109" s="37"/>
+    </row>
+    <row r="110" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N110" s="31"/>
+      <c r="O110" s="31"/>
+      <c r="P110" s="31"/>
+      <c r="Q110" s="37"/>
+      <c r="R110" s="37"/>
+    </row>
+    <row r="111" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N111" s="31"/>
+      <c r="O111" s="31"/>
+      <c r="P111" s="31"/>
+      <c r="Q111" s="37"/>
+      <c r="R111" s="37"/>
+    </row>
+    <row r="112" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N112" s="31"/>
+      <c r="O112" s="31"/>
+      <c r="P112" s="31"/>
+      <c r="Q112" s="37"/>
+      <c r="R112" s="37"/>
+    </row>
+    <row r="113" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N113" s="31"/>
+      <c r="O113" s="31"/>
+      <c r="P113" s="31"/>
+      <c r="Q113" s="37"/>
+      <c r="R113" s="37"/>
+    </row>
+    <row r="114" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N114" s="31"/>
+      <c r="O114" s="31"/>
+      <c r="P114" s="31"/>
+      <c r="Q114" s="37"/>
+      <c r="R114" s="37"/>
+    </row>
+    <row r="115" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N115" s="31"/>
+      <c r="O115" s="31"/>
+      <c r="P115" s="31"/>
+      <c r="Q115" s="37"/>
+      <c r="R115" s="37"/>
+    </row>
+    <row r="116" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N116" s="31"/>
+      <c r="O116" s="31"/>
+      <c r="P116" s="31"/>
+      <c r="Q116" s="37"/>
+      <c r="R116" s="37"/>
+    </row>
+    <row r="117" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N117" s="31"/>
+      <c r="O117" s="31"/>
+      <c r="P117" s="31"/>
+      <c r="Q117" s="37"/>
+      <c r="R117" s="37"/>
+    </row>
+    <row r="118" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N118" s="31"/>
+      <c r="O118" s="31"/>
+      <c r="P118" s="31"/>
+      <c r="Q118" s="37"/>
+      <c r="R118" s="37"/>
+    </row>
+    <row r="119" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N119" s="31"/>
+      <c r="O119" s="31"/>
+      <c r="P119" s="31"/>
+      <c r="Q119" s="37"/>
+      <c r="R119" s="37"/>
+    </row>
+    <row r="120" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N120" s="31"/>
+      <c r="O120" s="31"/>
+      <c r="P120" s="31"/>
+      <c r="Q120" s="37"/>
+      <c r="R120" s="37"/>
+    </row>
+    <row r="121" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N121" s="31"/>
+      <c r="O121" s="31"/>
+      <c r="P121" s="31"/>
+      <c r="Q121" s="37"/>
+      <c r="R121" s="37"/>
+    </row>
+    <row r="122" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N122" s="31"/>
+      <c r="O122" s="31"/>
+      <c r="P122" s="31"/>
+      <c r="Q122" s="37"/>
+      <c r="R122" s="37"/>
+    </row>
+    <row r="123" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N123" s="31"/>
+      <c r="O123" s="31"/>
+      <c r="P123" s="31"/>
+      <c r="Q123" s="37"/>
+      <c r="R123" s="37"/>
+    </row>
+    <row r="124" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N124" s="31"/>
+      <c r="O124" s="31"/>
+      <c r="P124" s="31"/>
+      <c r="Q124" s="37"/>
+      <c r="R124" s="37"/>
+    </row>
+    <row r="125" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N125" s="31"/>
+      <c r="O125" s="31"/>
+      <c r="P125" s="31"/>
+      <c r="Q125" s="37"/>
+      <c r="R125" s="37"/>
+    </row>
+    <row r="126" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N126" s="31"/>
+      <c r="O126" s="31"/>
+      <c r="P126" s="31"/>
+      <c r="Q126" s="37"/>
+      <c r="R126" s="37"/>
+    </row>
+    <row r="127" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N127" s="31"/>
+      <c r="O127" s="31"/>
+      <c r="P127" s="31"/>
+      <c r="Q127" s="37"/>
+      <c r="R127" s="37"/>
+    </row>
+    <row r="128" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N128" s="31"/>
+      <c r="O128" s="31"/>
+      <c r="P128" s="31"/>
+      <c r="Q128" s="37"/>
+      <c r="R128" s="37"/>
+    </row>
+    <row r="129" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N129" s="31"/>
+      <c r="O129" s="31"/>
+      <c r="P129" s="31"/>
+      <c r="Q129" s="37"/>
+      <c r="R129" s="37"/>
+    </row>
+    <row r="130" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N130" s="31"/>
+      <c r="O130" s="31"/>
+      <c r="P130" s="31"/>
+      <c r="Q130" s="37"/>
+      <c r="R130" s="37"/>
+    </row>
+    <row r="131" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N131" s="31"/>
+      <c r="O131" s="31"/>
+      <c r="P131" s="31"/>
+      <c r="Q131" s="37"/>
+      <c r="R131" s="37"/>
+    </row>
+    <row r="132" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N132" s="31"/>
+      <c r="O132" s="31"/>
+      <c r="P132" s="31"/>
+      <c r="Q132" s="37"/>
+      <c r="R132" s="37"/>
+    </row>
+    <row r="133" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N133" s="31"/>
+      <c r="O133" s="31"/>
+      <c r="P133" s="31"/>
+      <c r="Q133" s="37"/>
+      <c r="R133" s="37"/>
+    </row>
+    <row r="134" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N134" s="31"/>
+      <c r="O134" s="31"/>
+      <c r="P134" s="31"/>
+      <c r="Q134" s="37"/>
+      <c r="R134" s="37"/>
+    </row>
+    <row r="135" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N135" s="31"/>
+      <c r="O135" s="31"/>
+      <c r="P135" s="31"/>
+      <c r="Q135" s="37"/>
+      <c r="R135" s="37"/>
+    </row>
+    <row r="136" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N136" s="31"/>
+      <c r="O136" s="31"/>
+      <c r="P136" s="31"/>
+      <c r="Q136" s="37"/>
+      <c r="R136" s="37"/>
+    </row>
+    <row r="137" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N137" s="31"/>
+      <c r="O137" s="31"/>
+      <c r="P137" s="31"/>
+      <c r="Q137" s="37"/>
+      <c r="R137" s="37"/>
+    </row>
+    <row r="138" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N138" s="31"/>
+      <c r="O138" s="31"/>
+      <c r="P138" s="31"/>
+      <c r="Q138" s="37"/>
+      <c r="R138" s="37"/>
+    </row>
+    <row r="139" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N139" s="31"/>
+      <c r="O139" s="31"/>
+      <c r="P139" s="31"/>
+      <c r="Q139" s="37"/>
+      <c r="R139" s="37"/>
+    </row>
+    <row r="140" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N140" s="31"/>
+      <c r="O140" s="31"/>
+      <c r="P140" s="31"/>
+      <c r="Q140" s="37"/>
+      <c r="R140" s="37"/>
+    </row>
+    <row r="141" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N141" s="31"/>
+      <c r="O141" s="31"/>
+      <c r="P141" s="31"/>
+      <c r="Q141" s="37"/>
+      <c r="R141" s="37"/>
+    </row>
+    <row r="142" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N142" s="31"/>
+      <c r="O142" s="31"/>
+      <c r="P142" s="31"/>
+      <c r="Q142" s="37"/>
+      <c r="R142" s="37"/>
+    </row>
+    <row r="143" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N143" s="31"/>
+      <c r="O143" s="31"/>
+      <c r="P143" s="31"/>
+      <c r="Q143" s="37"/>
+      <c r="R143" s="37"/>
+    </row>
+    <row r="144" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N144" s="31"/>
+      <c r="O144" s="31"/>
+      <c r="P144" s="31"/>
+      <c r="Q144" s="37"/>
+      <c r="R144" s="37"/>
+    </row>
+    <row r="145" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N145" s="31"/>
+      <c r="O145" s="31"/>
+      <c r="P145" s="31"/>
+      <c r="Q145" s="37"/>
+      <c r="R145" s="37"/>
+    </row>
+    <row r="146" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N146" s="31"/>
+      <c r="O146" s="31"/>
+      <c r="P146" s="31"/>
+      <c r="Q146" s="37"/>
+      <c r="R146" s="37"/>
+    </row>
+    <row r="147" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N147" s="31"/>
+      <c r="O147" s="31"/>
+      <c r="P147" s="31"/>
+      <c r="Q147" s="37"/>
+      <c r="R147" s="37"/>
+    </row>
+    <row r="148" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N148" s="31"/>
+      <c r="O148" s="31"/>
+      <c r="P148" s="31"/>
+      <c r="Q148" s="37"/>
+      <c r="R148" s="37"/>
+    </row>
+    <row r="149" spans="14:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N149" s="31"/>
+      <c r="O149" s="31"/>
+      <c r="P149" s="37"/>
+      <c r="Q149" s="37"/>
+      <c r="R149" s="37"/>
+    </row>
+    <row r="150" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N150" s="37"/>
+      <c r="O150" s="37"/>
+      <c r="P150" s="37"/>
+      <c r="Q150" s="37"/>
+      <c r="R150" s="37"/>
+    </row>
+    <row r="151" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N151" s="37"/>
+      <c r="O151" s="37"/>
+      <c r="P151" s="37"/>
+      <c r="Q151" s="37"/>
+      <c r="R151" s="37"/>
+    </row>
+    <row r="152" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N152" s="37"/>
+      <c r="O152" s="37"/>
+      <c r="P152" s="37"/>
+      <c r="Q152" s="37"/>
+      <c r="R152" s="37"/>
+    </row>
+    <row r="153" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N153" s="37"/>
+      <c r="O153" s="37"/>
+      <c r="P153" s="37"/>
+      <c r="Q153" s="37"/>
+      <c r="R153" s="37"/>
+    </row>
+    <row r="154" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N154" s="37"/>
+      <c r="O154" s="37"/>
+      <c r="R154" s="37"/>
+    </row>
+    <row r="155" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R155" s="37"/>
+    </row>
+    <row r="156" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R156" s="37"/>
+    </row>
+    <row r="157" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R157" s="37"/>
+    </row>
+    <row r="158" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R158" s="37"/>
+    </row>
+    <row r="159" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R159" s="37"/>
+    </row>
+    <row r="160" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="R160" s="37"/>
+    </row>
+    <row r="161" spans="18:18" x14ac:dyDescent="0.35">
+      <c r="R161" s="37"/>
+    </row>
+    <row r="162" spans="18:18" x14ac:dyDescent="0.35">
+      <c r="R162" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>